<commit_message>
THW-0-F added to misbehaviour fouls
</commit_message>
<xml_diff>
--- a/stepout_qc_code/write_string/match_renum_detials.xlsx
+++ b/stepout_qc_code/write_string/match_renum_detials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rohit" sheetId="1" state="visible" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,6 +39,12 @@
       <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,7 +100,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -104,6 +110,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -471,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,7 +707,7 @@
       <c r="D9" t="n">
         <v>90</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F9" t="n">
@@ -724,7 +731,7 @@
       <c r="D10" t="n">
         <v>90</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F10" t="n">
@@ -750,7 +757,7 @@
           <t>Less than 60</t>
         </is>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F11" t="n">
@@ -774,11 +781,313 @@
       <c r="D12" t="n">
         <v>90</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="4" t="n">
         <v>45381</v>
       </c>
       <c r="F12" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mumbai City FC B</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U13</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1725</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hungry Hearts Soccer School U-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CFCI U13</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1797</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F14" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Roots FC U17</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Young Blues Elite FC U17</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1810</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F15" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mira Bhayander Football Club</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CFCI U13</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1802</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F16" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hungry Hearts Soccer school U15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bravo Football U15</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1695</v>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Footie First u13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>India Rush U13</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1798</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F18" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ajax JO17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CF Pachuca O17</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1837</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F19" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Masfout</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Gulf United FC</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1845</v>
+      </c>
+      <c r="D20" t="n">
+        <v>90</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F20" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ajax JO13-1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PSV O13</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1847</v>
+      </c>
+      <c r="D21" t="n">
+        <v>90</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Barca Academy Grana</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Footie First U-15</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1859</v>
+      </c>
+      <c r="D22" t="n">
+        <v>90</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F22" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mumbai City FC A U-15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Barca Academy Blau</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1879</v>
+      </c>
+      <c r="D23" t="n">
+        <v>90</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F23" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>NYN Sports Academy</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Hungry Hearts Soccer School U-13</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1868</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>45395</v>
+      </c>
+      <c r="F24" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +1101,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -969,11 +1278,233 @@
       <c r="D7" t="n">
         <v>90</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F7" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ajax JO14</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sparta U14</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1783</v>
+      </c>
+      <c r="D8" t="n">
+        <v>90</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hobro IK</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Naestved</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1794</v>
+      </c>
+      <c r="D9" t="n">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>45382</v>
+      </c>
+      <c r="F9" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hobro IK</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AC Horsens</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1793</v>
+      </c>
+      <c r="D10" t="n">
+        <v>90</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>45382</v>
+      </c>
+      <c r="F10" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FC Volendam U18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ajax U18</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1820</v>
+      </c>
+      <c r="D11" t="n">
+        <v>90</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F11" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Parikrama FC</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bangalore City FC A Div</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1790</v>
+      </c>
+      <c r="D12" t="n">
+        <v>90</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F12" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mira Road Youngsters FA U13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Barca Academy Blau U13</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1661</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ajax JO17</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PSG O17</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1838</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F14" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Feyenoord U16</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ajax U16</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1850</v>
+      </c>
+      <c r="D15" t="n">
+        <v>90</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Footie First U-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U15</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1862</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F16" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +1518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1218,7 +1749,7 @@
       <c r="D9" t="n">
         <v>90</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F9" t="n">
@@ -1242,7 +1773,7 @@
       <c r="D10" t="n">
         <v>90</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F10" t="n">
@@ -1266,10 +1797,288 @@
       <c r="D11" t="n">
         <v>90</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F11" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Soccerstar India</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mumbai Soccer Prodigies</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1703</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F12" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CFCI U13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mumbai Soccer Prodigies</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1813</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>VR Football Academy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Stellar Football Academy</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1803</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F14" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CFCI X U13</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1816</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Income Tax FC</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Blitz FC</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D16" t="n">
+        <v>90</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Income Tax FC</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sri Gajanana FC</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1832</v>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Ajax JO17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FK Partizan O17</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1835</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F18" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TSW White 2009</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sydney FC</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1842</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F19" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sporting Charleroi U14</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ajax U14</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1851</v>
+      </c>
+      <c r="D20" t="n">
+        <v>90</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F20" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Spurs Football Academy U-15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Barca Academy Grana</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1858</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F21" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ajax JO17-1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FC Volendam U17</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1877</v>
+      </c>
+      <c r="D22" t="n">
+        <v>90</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F22" t="n">
         <v>500</v>
       </c>
     </row>
@@ -1284,13 +2093,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="23.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -1583,7 +2392,7 @@
           <t>Less than 60</t>
         </is>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="4" t="n">
         <v>45379</v>
       </c>
       <c r="F12" t="n">
@@ -1607,15 +2416,292 @@
       <c r="D13" t="n">
         <v>90</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F13" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hobro IK</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>HB Koege</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1792</v>
+      </c>
+      <c r="D14" t="n">
+        <v>90</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F14" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Hobro IK</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sonderjyske</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1795</v>
+      </c>
+      <c r="D15" t="n">
+        <v>90</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mumbai City FC A U-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Mumbai City FC B U-15</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1806</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F16" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BTM FC</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bangalore City FC - A Div</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1833</v>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>45385</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>The Sports School U17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FX FA U17</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1809</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>45386</v>
+      </c>
+      <c r="F18" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ajax jo17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>fk partizan o17</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1839</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>45387</v>
+      </c>
+      <c r="F19" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TSP Red 2008</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Sydney FC</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1841</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>45389</v>
+      </c>
+      <c r="F20" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FC Utrecht JO15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ajax jo15</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1849</v>
+      </c>
+      <c r="D21" t="n">
+        <v>90</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>45391</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mumbai Soccer Prodigies U15</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Barca Academy Blau</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1861</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F22" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ajax JO14</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Feyenoord JO14</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1874</v>
+      </c>
+      <c r="D23" t="n">
+        <v>90</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>45393</v>
+      </c>
+      <c r="F23" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Jong Ajax U16 Women</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>IJburg U16 (f)</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1880</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F24" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1625,7 +2711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,7 +2846,7 @@
           <t>Less than 60</t>
         </is>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F5" t="n">
@@ -1784,11 +2870,63 @@
       <c r="D6" t="n">
         <v>90</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>45381</v>
       </c>
       <c r="F6" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Hungry Hearts Soccer School</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>D'Souza Football Academy A U-15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1771</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F7" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dsouza FA U13</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Footie First U13</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1843</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F8" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1802,7 +2940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1957,7 +3095,7 @@
       <c r="D6" t="n">
         <v>90</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F6" t="n">
@@ -1981,11 +3119,193 @@
       <c r="D7" t="n">
         <v>90</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="4" t="n">
         <v>45381</v>
       </c>
       <c r="F7" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MRUFC U17</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Young Blues Elite FC U17</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1787</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="F8" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mumbai Soccer Prodigies U15</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CFCI U15</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1807</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F9" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mumbai City FC B U13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Footie First</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F10" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Footie First U15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Spurs FA U15</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1656</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F11" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mumbai City FC A U13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Spurs FA U13</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1796</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F12" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mumbai City FC A U13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Barca Academy Blau U13</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1869</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SSE BFC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CFCI X Men U-13</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1864</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45395</v>
+      </c>
+      <c r="F14" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1999,7 +3319,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:F9"/>
@@ -2250,7 +3570,7 @@
       <c r="D10" t="n">
         <v>90</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F10" t="n">
@@ -2274,11 +3594,185 @@
       <c r="D11" t="n">
         <v>90</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="4" t="n">
         <v>45381</v>
       </c>
       <c r="F11" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Alchemy IFA U15</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Snipers FC A U15</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1422</v>
+      </c>
+      <c r="D12" t="n">
+        <v>90</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F12" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>VAS FA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Kickstart B</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1493</v>
+      </c>
+      <c r="D13" t="n">
+        <v>90</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F13" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>All stars A</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>All stars B</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1819</v>
+      </c>
+      <c r="D14" t="n">
+        <v>90</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F14" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Roots FC</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sreenidi Deccan</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1840</v>
+      </c>
+      <c r="D15" t="n">
+        <v>90</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mira Bhayander Football Club U13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Spurs Football Academy U13</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1734</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F16" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>All Stars Team A</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>All Stars Team B</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1854</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F17" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Barca Academy Grana U13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>VR Football Academy</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1865</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>45395</v>
+      </c>
+      <c r="F18" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2292,9 +3786,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2471,7 +3965,7 @@
       <c r="D7" t="n">
         <v>90</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F7" t="n">
@@ -2495,11 +3989,291 @@
       <c r="D8" t="n">
         <v>90</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F8" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Prime FA U17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Raman SA U17</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1786</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F9" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jong Ajax U16 Women</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>California U16</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1791</v>
+      </c>
+      <c r="D10" t="n">
+        <v>45</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F10" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Alchemy Ignis U17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Roots FC U17</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1788</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F11" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Alchemy Ignis U17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Raman SA U17</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1811</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F12" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mumbai City FC A U15</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Footie First U15</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1768</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SSE BFC U13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dsouza FA U13</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1799</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F14" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ajax JO17</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Manchester City O17</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1836</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FC Groningen U18</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ajax U18</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1846</v>
+      </c>
+      <c r="D16" t="n">
+        <v>90</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ajax JO13-2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam U13</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1848</v>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Alchemy Ignis U17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Young Blues Elite FC U17</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1873</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F18" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Soccerstar India</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Lemon Break U13</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1871</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>45395</v>
+      </c>
+      <c r="F19" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2513,7 +4287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2624,7 +4398,7 @@
           <t>Less than 60</t>
         </is>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="4" t="n">
         <v>45378</v>
       </c>
       <c r="F4" t="n">
@@ -2650,7 +4424,7 @@
           <t>Less than 60</t>
         </is>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>45380</v>
       </c>
       <c r="F5" t="n">
@@ -2674,10 +4448,284 @@
       <c r="D6" t="n">
         <v>90</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>45381</v>
       </c>
       <c r="F6" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mumbai Soccer Prodigies U15</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1657</v>
+      </c>
+      <c r="D7" t="n">
+        <v>90</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F7" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U15</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Spurs Football Academy U-15</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1770</v>
+      </c>
+      <c r="D8" t="n">
+        <v>90</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>45382</v>
+      </c>
+      <c r="F8" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U15</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>D'Souza Football Academy B U-15</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1808</v>
+      </c>
+      <c r="D9" t="n">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F9" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mira Road Youngsters FA U13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Soccerstar India U13</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1801</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F10" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hungry Hearts Soccer school U13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mira Road Youngsters FA U13</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1708</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F11" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mumbai city FC B U13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sporting Mumbai U13</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1815</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F12" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sporting Mumbai U13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RFYC Development Squad U13</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1726</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F13" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Gulf United FC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>City FC</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1852</v>
+      </c>
+      <c r="D14" t="n">
+        <v>90</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F14" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CFCI</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>D'Souza Football Academy A U-15</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1860</v>
+      </c>
+      <c r="D15" t="n">
+        <v>90</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>45392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Raman SA U17</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BBFS Residential Academy U17</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1872</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F16" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Barca Academy Grana</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>The Soccer Academy U15</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1878</v>
+      </c>
+      <c r="D17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>45395</v>
+      </c>
+      <c r="F17" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
multiple file loop done
</commit_message>
<xml_diff>
--- a/stepout_qc_code/write_string/match_renum_detials.xlsx
+++ b/stepout_qc_code/write_string/match_renum_detials.xlsx
@@ -3173,7 +3173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -4120,6 +4120,228 @@
         <v>45410</v>
       </c>
       <c r="F38" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam U15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Ajax JO15-1</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2037</v>
+      </c>
+      <c r="D39" t="n">
+        <v>90</v>
+      </c>
+      <c r="E39" s="6" t="n">
+        <v>45411</v>
+      </c>
+      <c r="F39" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Nita FA</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Pune Krida PA</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>90</v>
+      </c>
+      <c r="E40" s="6" t="n">
+        <v>45413</v>
+      </c>
+      <c r="F40" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Roots Red U15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Dash Athlectics U15</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2036</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E41" s="6" t="n">
+        <v>45414</v>
+      </c>
+      <c r="F41" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Young Blues Elite FC U17</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Raman SA U17</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2072</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>45416</v>
+      </c>
+      <c r="F42" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Ajax JO15-1</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Academy Fukushima U15</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2074</v>
+      </c>
+      <c r="D43" t="n">
+        <v>90</v>
+      </c>
+      <c r="E43" s="6" t="n">
+        <v>45417</v>
+      </c>
+      <c r="F43" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Loco. Tbilisi</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>FC Gareji Sagarejo</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>2089</v>
+      </c>
+      <c r="D44" t="n">
+        <v>90</v>
+      </c>
+      <c r="E44" s="6" t="n">
+        <v>45420</v>
+      </c>
+      <c r="F44" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>RFYC Development Squad</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Mumbai City FC B</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1991</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Less than 60</t>
+        </is>
+      </c>
+      <c r="E45" s="6" t="n">
+        <v>45421</v>
+      </c>
+      <c r="F45" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>FC Utrecht U17</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Ajax JO17-1</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>2097</v>
+      </c>
+      <c r="D46" t="n">
+        <v>90</v>
+      </c>
+      <c r="E46" s="6" t="n">
+        <v>45422</v>
+      </c>
+      <c r="F46" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Feyenoord O17</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Aax JO17-1</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2107</v>
+      </c>
+      <c r="D47" t="n">
+        <v>90</v>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>45425</v>
+      </c>
+      <c r="F47" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>